<commit_message>
update cost analysis and plexiglass dwg
</commit_message>
<xml_diff>
--- a/cost analysis/cost_analysis.xlsx
+++ b/cost analysis/cost_analysis.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
   <si>
     <t>Είδος</t>
   </si>
@@ -30,9 +30,6 @@
     <t>Τιμή (Euro)</t>
   </si>
   <si>
-    <t>Σύνολο (Euro)</t>
-  </si>
-  <si>
     <t>Τεμάχιο</t>
   </si>
   <si>
@@ -57,9 +54,6 @@
     <t>ΣΥΝΟΛΟ</t>
   </si>
   <si>
-    <t>Περίβλημα plexiglass</t>
-  </si>
-  <si>
     <t>Πυρήνας από κόντρα πλακέ θαλάσσης</t>
   </si>
   <si>
@@ -75,13 +69,31 @@
     <t>Power supply</t>
   </si>
   <si>
-    <t>Σύνολο (Euro) ver 2</t>
-  </si>
-  <si>
-    <t>Σύνολο (Euro) ver 3</t>
-  </si>
-  <si>
     <t>Πλακέτα Arduino ΟΝΕ</t>
+  </si>
+  <si>
+    <t>Σύνολο ver 2  (Euro) (1 τεμάχιο)</t>
+  </si>
+  <si>
+    <t>Σύνολο ver 3  (Euro) (1 τεμάχιο)</t>
+  </si>
+  <si>
+    <t>Σύνολο ver 1 (Euro) (1 τεμάχιο)</t>
+  </si>
+  <si>
+    <t>Σύνολο ver 2  (Euro) (10 τεμάχια)</t>
+  </si>
+  <si>
+    <t>Σύνολο ver 3  (Euro) (10 τεμάχια)</t>
+  </si>
+  <si>
+    <t>Περίβλημα plexiglass γαλακτερό 10mm</t>
+  </si>
+  <si>
+    <t>Σύνολο ver 1 (Euro) (10 τεμάχια)</t>
+  </si>
+  <si>
+    <t>Σύνολο (Euro) ver 1 (10 τεμάχια)</t>
   </si>
 </sst>
 </file>
@@ -123,7 +135,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -133,6 +145,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -235,7 +259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
@@ -273,9 +297,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -297,6 +318,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -603,12 +633,17 @@
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="7" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="11" max="11" width="21.7109375" customWidth="1"/>
+    <col min="12" max="12" width="20.85546875" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30.75" thickBot="1">
+    <row r="1" spans="1:13" ht="45.75" thickBot="1">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -621,74 +656,138 @@
       <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="30">
+      <c r="A2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>5</v>
       </c>
       <c r="C2" s="5">
         <v>1</v>
       </c>
       <c r="D2" s="4">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="E2" s="5">
-        <f t="shared" ref="E2:F4" si="0">C2*D2</f>
-        <v>150</v>
+        <f t="shared" ref="E2:E4" si="0">C2*D2</f>
+        <v>250</v>
       </c>
       <c r="F2" s="6">
         <f t="shared" ref="F2:G8" si="1">E2</f>
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="G2" s="6">
         <f t="shared" si="1"/>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="17" t="s">
+        <v>250</v>
+      </c>
+      <c r="H2">
+        <v>230</v>
+      </c>
+      <c r="I2">
+        <f t="shared" ref="I2:I9" si="2">H2</f>
+        <v>230</v>
+      </c>
+      <c r="J2">
+        <f>H2</f>
+        <v>230</v>
+      </c>
+      <c r="K2">
+        <v>200</v>
+      </c>
+      <c r="L2">
+        <f t="shared" ref="L2:L9" si="3">K2</f>
+        <v>200</v>
+      </c>
+      <c r="M2">
+        <f>K2</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="17">
+      <c r="B3" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="16">
         <v>1</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="16">
         <v>70</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="16">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="17">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
-      <c r="G3" s="18">
-        <f t="shared" ref="G3" si="2">F3</f>
+      <c r="G3" s="17">
+        <f t="shared" ref="G3" si="4">F3</f>
         <v>70</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="30">
+      <c r="H3" s="17">
+        <f>D3</f>
+        <v>70</v>
+      </c>
+      <c r="I3" s="17">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="J3" s="17">
+        <f>I3</f>
+        <v>70</v>
+      </c>
+      <c r="K3" s="17">
+        <f>G3</f>
+        <v>70</v>
+      </c>
+      <c r="L3" s="17">
+        <f t="shared" si="3"/>
+        <v>70</v>
+      </c>
+      <c r="M3" s="17">
+        <f>L3</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="30">
       <c r="A4" s="11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -705,42 +804,90 @@
         <v>25</v>
       </c>
       <c r="G4" s="3">
-        <f t="shared" ref="G4" si="3">F4</f>
+        <f t="shared" ref="G4" si="5">F4</f>
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="17">
+      <c r="H4">
+        <f>D4</f>
+        <v>25</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="J4">
+        <f>H4</f>
+        <v>25</v>
+      </c>
+      <c r="K4">
+        <f>G4</f>
+        <v>25</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="M4">
+        <f>K4</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="17">
+      <c r="C5" s="16">
+        <v>4</v>
+      </c>
+      <c r="D5" s="16">
         <v>12</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="16">
         <f>C5*D5</f>
         <v>48</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="17">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="G5" s="18">
-        <f t="shared" ref="G5" si="4">F5</f>
+      <c r="G5" s="17">
+        <f t="shared" ref="G5" si="6">F5</f>
         <v>48</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5" s="17">
+        <f t="shared" ref="H5:H10" si="7">E5</f>
+        <v>48</v>
+      </c>
+      <c r="I5" s="17">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="J5" s="17">
+        <f>H5</f>
+        <v>48</v>
+      </c>
+      <c r="K5" s="17">
+        <f t="shared" ref="K5:K10" si="8">H5</f>
+        <v>48</v>
+      </c>
+      <c r="L5" s="17">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="M5" s="17">
+        <f>K5</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -757,42 +904,90 @@
         <v>10</v>
       </c>
       <c r="G6" s="3">
-        <f t="shared" ref="G6" si="5">F6</f>
+        <f t="shared" ref="G6" si="9">F6</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="17">
+      <c r="H6">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="J6">
+        <f>H6</f>
+        <v>10</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="M6">
+        <f>K6</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="16">
         <v>1</v>
       </c>
-      <c r="D7" s="17">
-        <v>30</v>
-      </c>
-      <c r="E7" s="17">
-        <f t="shared" ref="E7:F10" si="6">C7*D7</f>
-        <v>30</v>
-      </c>
-      <c r="F7" s="18">
+      <c r="D7" s="16">
+        <v>30</v>
+      </c>
+      <c r="E7" s="16">
+        <f t="shared" ref="E7:E10" si="10">C7*D7</f>
+        <v>30</v>
+      </c>
+      <c r="F7" s="17">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="G7" s="18">
-        <f t="shared" ref="G7" si="7">F7</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="30">
+      <c r="G7" s="17">
+        <f t="shared" ref="G7" si="11">F7</f>
+        <v>30</v>
+      </c>
+      <c r="H7" s="17">
+        <f t="shared" si="7"/>
+        <v>30</v>
+      </c>
+      <c r="I7" s="17">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="J7" s="17">
+        <f>I7</f>
+        <v>30</v>
+      </c>
+      <c r="K7" s="17">
+        <f t="shared" si="8"/>
+        <v>30</v>
+      </c>
+      <c r="L7" s="17">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="M7" s="17">
+        <f>L7</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="30">
       <c r="A8" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="1">
         <v>6</v>
@@ -801,7 +996,7 @@
         <v>5</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>30</v>
       </c>
       <c r="F8" s="3">
@@ -809,42 +1004,90 @@
         <v>30</v>
       </c>
       <c r="G8" s="3">
-        <f t="shared" ref="G8" si="8">F8</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="17">
+        <f t="shared" ref="G8" si="12">F8</f>
+        <v>30</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="7"/>
+        <v>30</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="J8">
+        <f>H8</f>
+        <v>30</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="8"/>
+        <v>30</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="M8">
+        <f>K8</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="16">
         <v>1</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="16">
         <v>20</v>
       </c>
-      <c r="E9" s="17">
-        <f t="shared" ref="E9" si="9">C9*D9</f>
+      <c r="E9" s="16">
+        <f t="shared" ref="E9" si="13">C9*D9</f>
         <v>20</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="17">
         <f>E9</f>
         <v>20</v>
       </c>
-      <c r="G9" s="18">
-        <f t="shared" ref="G9" si="10">F9</f>
+      <c r="G9" s="17">
+        <f t="shared" ref="G9" si="14">F9</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1">
+      <c r="H9" s="17">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="I9" s="17">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="J9" s="17">
+        <f>H9</f>
+        <v>20</v>
+      </c>
+      <c r="K9" s="17">
+        <f t="shared" si="8"/>
+        <v>20</v>
+      </c>
+      <c r="L9" s="17">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="M9" s="17">
+        <f>K9</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15" customHeight="1">
       <c r="A10" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" s="1">
         <v>1</v>
@@ -853,28 +1096,46 @@
         <v>240</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>240</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A11" s="16" t="s">
+      <c r="H10">
+        <f t="shared" si="7"/>
+        <v>240</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="8"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A11" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="18"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="M11" s="17"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="11" t="s">
         <v>9</v>
-      </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="18"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="11" t="s">
-        <v>10</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="1">
@@ -886,23 +1147,41 @@
         <v>180</v>
       </c>
       <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1">
+      <c r="I12">
+        <f>F12</f>
+        <v>180</v>
+      </c>
+      <c r="L12">
+        <f>I12</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="18"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15.75" thickBot="1">
       <c r="A14" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="8">
@@ -914,30 +1193,62 @@
       <c r="G14" s="8">
         <v>180</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" thickBot="1">
-      <c r="A15" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
+      <c r="J14">
+        <f>G14</f>
+        <v>180</v>
+      </c>
+      <c r="M14">
+        <f>J14</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15" customHeight="1" thickBot="1">
+      <c r="A15" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="20"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
       <c r="E15" s="14">
-        <f>SUM(E2:E14)</f>
-        <v>623</v>
-      </c>
-      <c r="F15" s="23">
-        <f>SUM(F2:F14)</f>
-        <v>563</v>
-      </c>
-      <c r="G15" s="24">
-        <f>SUM(G2:G14)</f>
-        <v>563</v>
+        <f t="shared" ref="E15:M15" si="15">SUM(E2:E14)</f>
+        <v>723</v>
+      </c>
+      <c r="F15" s="22">
+        <f t="shared" si="15"/>
+        <v>663</v>
+      </c>
+      <c r="G15" s="22">
+        <f t="shared" si="15"/>
+        <v>663</v>
+      </c>
+      <c r="H15" s="22">
+        <f t="shared" si="15"/>
+        <v>703</v>
+      </c>
+      <c r="I15" s="22">
+        <f t="shared" si="15"/>
+        <v>643</v>
+      </c>
+      <c r="J15" s="22">
+        <f t="shared" si="15"/>
+        <v>643</v>
+      </c>
+      <c r="K15" s="22">
+        <f t="shared" si="15"/>
+        <v>673</v>
+      </c>
+      <c r="L15" s="22">
+        <f t="shared" si="15"/>
+        <v>613</v>
+      </c>
+      <c r="M15" s="23">
+        <f t="shared" si="15"/>
+        <v>613</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="50" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update section and cost analysis
</commit_message>
<xml_diff>
--- a/cost analysis/cost_analysis.xlsx
+++ b/cost analysis/cost_analysis.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
   <si>
     <t>Είδος</t>
   </si>
@@ -93,7 +93,13 @@
     <t>Σύνολο ver 1 (Euro) (10 τεμάχια)</t>
   </si>
   <si>
-    <t>Σύνολο (Euro) ver 1 (10 τεμάχια)</t>
+    <t>Σύνολο (Euro) ver 1 (100 τεμάχια)</t>
+  </si>
+  <si>
+    <t>Σύνολο ver 2  (Euro) (100 τεμάχια)</t>
+  </si>
+  <si>
+    <t>Σύνολο ver 3  (Euro) (100 τεμάχια)</t>
   </si>
 </sst>
 </file>
@@ -161,7 +167,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -184,82 +190,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
@@ -268,34 +203,8 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -307,26 +216,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,7 +526,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -633,157 +535,157 @@
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
     <col min="6" max="7" width="17.28515625" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" customWidth="1"/>
+    <col min="9" max="9" width="21" customWidth="1"/>
     <col min="10" max="10" width="20.7109375" customWidth="1"/>
     <col min="11" max="11" width="21.7109375" customWidth="1"/>
     <col min="12" max="12" width="20.85546875" customWidth="1"/>
-    <col min="13" max="13" width="18.85546875" customWidth="1"/>
+    <col min="13" max="13" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="45.75" thickBot="1">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:13" ht="45">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="K1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="M1" s="26" t="s">
-        <v>22</v>
+      <c r="L1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="30">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="1">
         <v>1</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="2">
         <v>250</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="1">
         <f t="shared" ref="E2:E4" si="0">C2*D2</f>
         <v>250</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="3">
         <f t="shared" ref="F2:G8" si="1">E2</f>
         <v>250</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="3">
         <f t="shared" si="1"/>
         <v>250</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="3">
         <v>230</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="3">
         <f t="shared" ref="I2:I9" si="2">H2</f>
         <v>230</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="3">
         <f>H2</f>
         <v>230</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="3">
         <v>200</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="3">
         <f t="shared" ref="L2:L9" si="3">K2</f>
         <v>200</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="3">
         <f>K2</f>
         <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="6">
         <v>1</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="6">
         <v>70</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="6">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="7">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
-      <c r="G3" s="17">
+      <c r="G3" s="7">
         <f t="shared" ref="G3" si="4">F3</f>
         <v>70</v>
       </c>
-      <c r="H3" s="17">
+      <c r="H3" s="7">
         <f>D3</f>
         <v>70</v>
       </c>
-      <c r="I3" s="17">
+      <c r="I3" s="7">
         <f t="shared" si="2"/>
         <v>70</v>
       </c>
-      <c r="J3" s="17">
+      <c r="J3" s="7">
         <f>I3</f>
         <v>70</v>
       </c>
-      <c r="K3" s="17">
+      <c r="K3" s="7">
         <f>G3</f>
         <v>70</v>
       </c>
-      <c r="L3" s="17">
+      <c r="L3" s="7">
         <f t="shared" si="3"/>
         <v>70</v>
       </c>
-      <c r="M3" s="17">
+      <c r="M3" s="7">
         <f>L3</f>
         <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="30">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -807,83 +709,83 @@
         <f t="shared" ref="G4" si="5">F4</f>
         <v>25</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="3">
         <f>D4</f>
         <v>25</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="3">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="3">
         <f>H4</f>
         <v>25</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="3">
         <f>G4</f>
         <v>25</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="3">
         <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="3">
         <f>K4</f>
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="6">
         <v>4</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="6">
         <v>12</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="6">
         <f>C5*D5</f>
         <v>48</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="7">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="G5" s="17">
+      <c r="G5" s="7">
         <f t="shared" ref="G5" si="6">F5</f>
         <v>48</v>
       </c>
-      <c r="H5" s="17">
+      <c r="H5" s="7">
         <f t="shared" ref="H5:H10" si="7">E5</f>
         <v>48</v>
       </c>
-      <c r="I5" s="17">
+      <c r="I5" s="7">
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
-      <c r="J5" s="17">
+      <c r="J5" s="7">
         <f>H5</f>
         <v>48</v>
       </c>
-      <c r="K5" s="17">
+      <c r="K5" s="7">
         <f t="shared" ref="K5:K10" si="8">H5</f>
         <v>48</v>
       </c>
-      <c r="L5" s="17">
+      <c r="L5" s="7">
         <f t="shared" si="3"/>
         <v>48</v>
       </c>
-      <c r="M5" s="17">
+      <c r="M5" s="7">
         <f>K5</f>
         <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -907,83 +809,83 @@
         <f t="shared" ref="G6" si="9">F6</f>
         <v>10</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="3">
         <f t="shared" si="7"/>
         <v>10</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="3">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="3">
         <f>H6</f>
         <v>10</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="3">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="3">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="3">
         <f>K6</f>
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="6">
         <v>1</v>
       </c>
-      <c r="D7" s="16">
-        <v>30</v>
-      </c>
-      <c r="E7" s="16">
+      <c r="D7" s="6">
+        <v>30</v>
+      </c>
+      <c r="E7" s="6">
         <f t="shared" ref="E7:E10" si="10">C7*D7</f>
         <v>30</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="7">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="G7" s="17">
+      <c r="G7" s="7">
         <f t="shared" ref="G7" si="11">F7</f>
         <v>30</v>
       </c>
-      <c r="H7" s="17">
+      <c r="H7" s="7">
         <f t="shared" si="7"/>
         <v>30</v>
       </c>
-      <c r="I7" s="17">
+      <c r="I7" s="7">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="J7" s="17">
+      <c r="J7" s="7">
         <f>I7</f>
         <v>30</v>
       </c>
-      <c r="K7" s="17">
+      <c r="K7" s="7">
         <f t="shared" si="8"/>
         <v>30</v>
       </c>
-      <c r="L7" s="17">
+      <c r="L7" s="7">
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="M7" s="17">
+      <c r="M7" s="7">
         <f>L7</f>
         <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="30">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1007,83 +909,83 @@
         <f t="shared" ref="G8" si="12">F8</f>
         <v>30</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="3">
         <f t="shared" si="7"/>
         <v>30</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="3">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="3">
         <f>H8</f>
         <v>30</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="3">
         <f t="shared" si="8"/>
         <v>30</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="3">
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="3">
         <f>K8</f>
         <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="6">
         <v>1</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="6">
         <v>20</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="6">
         <f t="shared" ref="E9" si="13">C9*D9</f>
         <v>20</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="7">
         <f>E9</f>
         <v>20</v>
       </c>
-      <c r="G9" s="17">
+      <c r="G9" s="7">
         <f t="shared" ref="G9" si="14">F9</f>
         <v>20</v>
       </c>
-      <c r="H9" s="17">
+      <c r="H9" s="7">
         <f t="shared" si="7"/>
         <v>20</v>
       </c>
-      <c r="I9" s="17">
+      <c r="I9" s="7">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="J9" s="17">
+      <c r="J9" s="7">
         <f>H9</f>
         <v>20</v>
       </c>
-      <c r="K9" s="17">
+      <c r="K9" s="7">
         <f t="shared" si="8"/>
         <v>20</v>
       </c>
-      <c r="L9" s="17">
+      <c r="L9" s="7">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="M9" s="17">
+      <c r="M9" s="7">
         <f>K9</f>
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15" customHeight="1">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1101,40 +1003,44 @@
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10">
+      <c r="H10" s="3">
         <f t="shared" si="7"/>
         <v>240</v>
       </c>
-      <c r="K10">
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3">
         <f t="shared" si="8"/>
         <v>240</v>
       </c>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
     </row>
     <row r="11" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17" t="s">
+      <c r="B11" s="8"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17" t="s">
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17" t="s">
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="M11" s="17"/>
+      <c r="M11" s="7"/>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="2"/>
@@ -1147,101 +1053,109 @@
         <v>180</v>
       </c>
       <c r="G12" s="3"/>
-      <c r="I12">
+      <c r="H12" s="3"/>
+      <c r="I12" s="3">
         <f>F12</f>
         <v>180</v>
       </c>
-      <c r="L12">
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3">
         <f>I12</f>
         <v>180</v>
       </c>
+      <c r="M12" s="3"/>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="16" t="s">
+      <c r="B13" s="8"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16" t="s">
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16" t="s">
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A14" s="12" t="s">
+    <row r="14" spans="1:13">
+      <c r="A14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8">
+      <c r="B14" s="2"/>
+      <c r="C14" s="1">
         <v>1</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="8">
+      <c r="D14" s="1"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="1">
         <v>180</v>
       </c>
-      <c r="J14">
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3">
         <f>G14</f>
         <v>180</v>
       </c>
-      <c r="M14">
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3">
         <f>J14</f>
         <v>180</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15" customHeight="1" thickBot="1">
-      <c r="A15" s="19" t="s">
+    <row r="15" spans="1:13" ht="15" customHeight="1">
+      <c r="A15" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="14">
+      <c r="B15" s="8"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="9">
         <f t="shared" ref="E15:M15" si="15">SUM(E2:E14)</f>
         <v>723</v>
       </c>
-      <c r="F15" s="22">
+      <c r="F15" s="13">
         <f t="shared" si="15"/>
         <v>663</v>
       </c>
-      <c r="G15" s="22">
+      <c r="G15" s="13">
         <f t="shared" si="15"/>
         <v>663</v>
       </c>
-      <c r="H15" s="22">
+      <c r="H15" s="13">
         <f t="shared" si="15"/>
         <v>703</v>
       </c>
-      <c r="I15" s="22">
+      <c r="I15" s="13">
         <f t="shared" si="15"/>
         <v>643</v>
       </c>
-      <c r="J15" s="22">
+      <c r="J15" s="13">
         <f t="shared" si="15"/>
         <v>643</v>
       </c>
-      <c r="K15" s="22">
+      <c r="K15" s="13">
         <f t="shared" si="15"/>
         <v>673</v>
       </c>
-      <c r="L15" s="22">
+      <c r="L15" s="13">
         <f t="shared" si="15"/>
         <v>613</v>
       </c>
-      <c r="M15" s="23">
+      <c r="M15" s="13">
         <f t="shared" si="15"/>
         <v>613</v>
       </c>

</xml_diff>

<commit_message>
more images & updated cost
</commit_message>
<xml_diff>
--- a/cost analysis/cost_analysis.xlsx
+++ b/cost analysis/cost_analysis.xlsx
@@ -33,9 +33,6 @@
     <t>Τεμάχιο</t>
   </si>
   <si>
-    <t>Μεταλλική βάση</t>
-  </si>
-  <si>
     <t xml:space="preserve">τεμάχιο </t>
   </si>
   <si>
@@ -100,6 +97,9 @@
   </si>
   <si>
     <t>Σύνολο ver 3  (Euro) (100 τεμάχια)</t>
+  </si>
+  <si>
+    <t>Μεταλλική βάση (γαλβανισμένη με ηλεκτροστατική βαφή)</t>
   </si>
 </sst>
 </file>
@@ -525,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -545,7 +545,7 @@
     <col min="13" max="13" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="45">
+    <row r="1" spans="1:13" ht="30">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -559,36 +559,36 @@
         <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="10" t="s">
+      <c r="J1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" s="11" t="s">
+      <c r="L1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>26</v>
-      </c>
-      <c r="M1" s="11" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="30">
       <c r="A2" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
@@ -634,9 +634,9 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" ht="30">
       <c r="A3" s="5" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>4</v>
@@ -645,51 +645,49 @@
         <v>1</v>
       </c>
       <c r="D3" s="6">
-        <v>70</v>
+        <v>315</v>
       </c>
       <c r="E3" s="6">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>315</v>
       </c>
       <c r="F3" s="7">
         <f t="shared" si="1"/>
-        <v>70</v>
+        <v>315</v>
       </c>
       <c r="G3" s="7">
         <f t="shared" ref="G3" si="4">F3</f>
-        <v>70</v>
+        <v>315</v>
       </c>
       <c r="H3" s="7">
-        <f>D3</f>
-        <v>70</v>
+        <v>115</v>
       </c>
       <c r="I3" s="7">
         <f t="shared" si="2"/>
-        <v>70</v>
+        <v>115</v>
       </c>
       <c r="J3" s="7">
         <f>I3</f>
-        <v>70</v>
+        <v>115</v>
       </c>
       <c r="K3" s="7">
-        <f>G3</f>
-        <v>70</v>
+        <v>107</v>
       </c>
       <c r="L3" s="7">
         <f t="shared" si="3"/>
-        <v>70</v>
+        <v>107</v>
       </c>
       <c r="M3" s="7">
         <f>L3</f>
-        <v>70</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="30">
       <c r="A4" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -736,7 +734,7 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>4</v>
@@ -786,7 +784,7 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
@@ -836,7 +834,7 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>4</v>
@@ -886,7 +884,7 @@
     </row>
     <row r="8" spans="1:13" ht="30">
       <c r="A8" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>4</v>
@@ -936,7 +934,7 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>4</v>
@@ -986,7 +984,7 @@
     </row>
     <row r="10" spans="1:13" ht="15" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>4</v>
@@ -1018,30 +1016,30 @@
     </row>
     <row r="11" spans="1:13" ht="15.75" customHeight="1">
       <c r="A11" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
       <c r="L11" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M11" s="7"/>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="1">
@@ -1068,7 +1066,7 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="6"/>
@@ -1076,22 +1074,22 @@
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
       <c r="M13" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="1">
@@ -1118,46 +1116,46 @@
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1">
       <c r="A15" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="9">
         <f t="shared" ref="E15:M15" si="15">SUM(E2:E14)</f>
-        <v>723</v>
+        <v>968</v>
       </c>
       <c r="F15" s="13">
         <f t="shared" si="15"/>
-        <v>663</v>
+        <v>908</v>
       </c>
       <c r="G15" s="13">
         <f t="shared" si="15"/>
-        <v>663</v>
+        <v>908</v>
       </c>
       <c r="H15" s="13">
         <f t="shared" si="15"/>
-        <v>703</v>
+        <v>748</v>
       </c>
       <c r="I15" s="13">
         <f t="shared" si="15"/>
-        <v>643</v>
+        <v>688</v>
       </c>
       <c r="J15" s="13">
         <f t="shared" si="15"/>
-        <v>643</v>
+        <v>688</v>
       </c>
       <c r="K15" s="13">
         <f t="shared" si="15"/>
-        <v>673</v>
+        <v>710</v>
       </c>
       <c r="L15" s="13">
         <f t="shared" si="15"/>
-        <v>613</v>
+        <v>650</v>
       </c>
       <c r="M15" s="13">
         <f t="shared" si="15"/>
-        <v>613</v>
+        <v>650</v>
       </c>
     </row>
   </sheetData>

</xml_diff>